<commit_message>
Completed part with downloading the list of items
</commit_message>
<xml_diff>
--- a/Shop/Files/qwerty.xlsx
+++ b/Shop/Files/qwerty.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>NoImage.jpg</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Some description6</t>
+  </si>
+  <si>
+    <t>hgfjf</t>
+  </si>
+  <si>
+    <t>sfvdf</t>
+  </si>
+  <si>
+    <t>фитнесс</t>
   </si>
 </sst>
 </file>
@@ -387,113 +396,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="B8:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1">
+    <row r="8" spans="2:6">
+      <c r="B8">
+        <v>999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9">
         <v>1000</v>
       </c>
-      <c r="B1">
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+    <row r="10" spans="2:6">
+      <c r="B10">
         <v>1001</v>
       </c>
-      <c r="B2">
+      <c r="C10">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
+    <row r="11" spans="2:6">
+      <c r="B11">
         <v>1002</v>
       </c>
-      <c r="B3">
+      <c r="C11">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4">
+    <row r="12" spans="2:6">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
+    <row r="13" spans="2:6">
+      <c r="B13">
         <v>1004</v>
       </c>
-      <c r="B5">
+      <c r="C13">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D13" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
+    <row r="14" spans="2:6">
+      <c r="B14">
         <v>1005</v>
       </c>
-      <c r="B6">
+      <c r="C14">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D14" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E14" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F14" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>